<commit_message>
Updating figures for GxE comparison
</commit_message>
<xml_diff>
--- a/notes/variety maturity classification.xlsx
+++ b/notes/variety maturity classification.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive-110536913573078057504/My Drive/Research/Publications/Chapter 4/Version 2/GitHub/cndc_bayesian_eval/notes/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Volumes/GoogleDrive/My Drive/Research/Publications/Chapter 4/Version 2/GitHub/cndc_bayesian_eval/notes/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C09A37A9-A96E-E745-A1C2-BECEC9570671}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47185DC3-2BD4-764A-B82F-57AA2AE3CEBD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13180" yWindow="500" windowWidth="15620" windowHeight="16260" xr2:uid="{13740538-63D8-AE47-B5A7-1DD91467E65C}"/>
+    <workbookView xWindow="26820" yWindow="500" windowWidth="14140" windowHeight="16260" xr2:uid="{13740538-63D8-AE47-B5A7-1DD91467E65C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -576,7 +576,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>